<commit_message>
Added some peel info to flux processing
</commit_message>
<xml_diff>
--- a/TUFLOWFV/miscellaneous/nodestring_importing/Flux Order WQ 1.xlsx
+++ b/TUFLOWFV/miscellaneous/nodestring_importing/Flux Order WQ 1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Cloudstor\Data_Lowerlakes\Sim Processing\CEWH 2017\Flux Processing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Flux Processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,91 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="55">
+  <si>
+    <t>Header</t>
+  </si>
+  <si>
+    <t>Flow</t>
+  </si>
+  <si>
+    <t>Salt</t>
+  </si>
+  <si>
+    <t>Temp</t>
+  </si>
+  <si>
+    <t>Trace_1</t>
+  </si>
+  <si>
+    <t>m^3/s</t>
+  </si>
+  <si>
+    <t>psu m^3/2</t>
+  </si>
+  <si>
+    <t>C m^3/s</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>mmol / s</t>
+  </si>
+  <si>
+    <t>Conversion Equation</t>
+  </si>
+  <si>
+    <t>Final Units</t>
+  </si>
+  <si>
+    <t>Initial Units</t>
+  </si>
+  <si>
+    <t>C m^3</t>
+  </si>
+  <si>
+    <t>m^3</t>
+  </si>
+  <si>
+    <t>Tonnes</t>
+  </si>
+  <si>
+    <t>1/1000</t>
+  </si>
+  <si>
+    <t>Conversion Factor (to Tonnes)</t>
+  </si>
+  <si>
+    <t>32 / (1000*1000*1000)</t>
+  </si>
+  <si>
+    <t>28.1/(1000*1000*1000)</t>
+  </si>
+  <si>
+    <t>14/(1000*1000*1000)</t>
+  </si>
+  <si>
+    <t>31/(1000*1000*1000)</t>
+  </si>
+  <si>
+    <t>12/(1000*1000*1000)</t>
+  </si>
+  <si>
+    <t>(12/50) / (1000*1000*1000)</t>
+  </si>
+  <si>
+    <t>tonnes</t>
+  </si>
+  <si>
+    <t>TRC_age</t>
+  </si>
+  <si>
+    <t>NCS_ss1</t>
+  </si>
+  <si>
+    <t>NCS_ss2</t>
+  </si>
   <si>
     <t>OXY_oxy</t>
   </si>
@@ -41,6 +125,15 @@
     <t>PHS_frp</t>
   </si>
   <si>
+    <t>PHS_frp_ads</t>
+  </si>
+  <si>
+    <t>OGM_doc</t>
+  </si>
+  <si>
+    <t>OGM_poc</t>
+  </si>
+  <si>
     <t>OGM_don</t>
   </si>
   <si>
@@ -53,97 +146,49 @@
     <t>OGM_pop</t>
   </si>
   <si>
-    <t>OGM_doc</t>
-  </si>
-  <si>
-    <t>OGM_poc</t>
+    <t>OGM_docr</t>
+  </si>
+  <si>
+    <t>OGM_donr</t>
+  </si>
+  <si>
+    <t>OGM_dopr</t>
+  </si>
+  <si>
+    <t>OGM_cpom</t>
   </si>
   <si>
     <t>PHY_grn</t>
   </si>
   <si>
-    <t>Header</t>
-  </si>
-  <si>
-    <t>Flow</t>
-  </si>
-  <si>
-    <t>Salt</t>
-  </si>
-  <si>
-    <t>Temp</t>
-  </si>
-  <si>
-    <t>Trace_1</t>
-  </si>
-  <si>
-    <t>m^3/s</t>
-  </si>
-  <si>
-    <t>psu m^3/2</t>
-  </si>
-  <si>
-    <t>C m^3/s</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>mmol / s</t>
-  </si>
-  <si>
-    <t>Conversion Equation</t>
-  </si>
-  <si>
-    <t>Final Units</t>
-  </si>
-  <si>
-    <t>Initial Units</t>
-  </si>
-  <si>
-    <t>C m^3</t>
-  </si>
-  <si>
-    <t>m^3</t>
-  </si>
-  <si>
-    <t>Tonnes</t>
-  </si>
-  <si>
-    <t>1/1000</t>
-  </si>
-  <si>
-    <t>Conversion Factor (to Tonnes)</t>
-  </si>
-  <si>
-    <t>32 / (1000*1000*1000)</t>
-  </si>
-  <si>
-    <t>28.1/(1000*1000*1000)</t>
-  </si>
-  <si>
-    <t>14/(1000*1000*1000)</t>
-  </si>
-  <si>
-    <t>31/(1000*1000*1000)</t>
-  </si>
-  <si>
-    <t>12/(1000*1000*1000)</t>
-  </si>
-  <si>
-    <t>(12/50) / (1000*1000*1000)</t>
-  </si>
-  <si>
-    <t>tonnes</t>
-  </si>
-  <si>
-    <t>PHS_frp_ads</t>
-  </si>
-  <si>
-    <t>TRC_age</t>
-  </si>
-  <si>
-    <t>TRC_ss1</t>
+    <t>PHY_crypt</t>
+  </si>
+  <si>
+    <t>PHY_diatom</t>
+  </si>
+  <si>
+    <t>PHY_dino</t>
+  </si>
+  <si>
+    <t>PHY_dino_IN</t>
+  </si>
+  <si>
+    <t>PHY_bga</t>
+  </si>
+  <si>
+    <t>PHY_bga_rho</t>
+  </si>
+  <si>
+    <t>MAG_chaetomorpha</t>
+  </si>
+  <si>
+    <t>MAG_chaetomorpha_IN</t>
+  </si>
+  <si>
+    <t>MAG_chaetomorpha_IP</t>
+  </si>
+  <si>
+    <t>BIV_filtfrac</t>
   </si>
 </sst>
 </file>
@@ -223,7 +268,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -234,11 +279,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -521,15 +561,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.453125" bestFit="1" customWidth="1"/>
@@ -547,30 +587,30 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="C1" s="3" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -581,31 +621,31 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D3" s="2">
         <f>1/1000</f>
         <v>1E-3</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
@@ -616,13 +656,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
@@ -632,349 +672,535 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>38</v>
+      <c r="A6" t="s">
+        <v>25</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>39</v>
+      <c r="A7" t="s">
+        <v>26</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>0</v>
+      <c r="A8" t="s">
+        <v>27</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="D8" s="2">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="2">
         <f>32 / (1000*1000*1000)</f>
         <v>3.2000000000000002E-8</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="2">
+      <c r="E9" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="2">
         <f>28.1/(1000*1000*1000)</f>
         <v>2.81E-8</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="2">
-        <f>14/(1000*1000*1000)</f>
-        <v>1.4E-8</v>
-      </c>
       <c r="E10" s="2" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>3</v>
+      <c r="A11" t="s">
+        <v>30</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D11" s="2">
         <f>14/(1000*1000*1000)</f>
         <v>1.4E-8</v>
       </c>
       <c r="E11" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="2">
+        <f>14/(1000*1000*1000)</f>
+        <v>1.4E-8</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="2">
-        <f>31/(1000*1000*1000)</f>
-        <v>3.1E-8</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="B13" s="1" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D13" s="2">
         <f>31/(1000*1000*1000)</f>
         <v>3.1E-8</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="B14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="2">
+        <f>31/(1000*1000*1000)</f>
+        <v>3.1E-8</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="2">
-        <f>12/(1000*1000*1000)</f>
-        <v>1.2E-8</v>
-      </c>
-      <c r="E14" s="2" t="s">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="B15" s="1" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D15" s="2">
         <f>12/(1000*1000*1000)</f>
         <v>1.2E-8</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
-        <v>5</v>
+      <c r="A16" t="s">
+        <v>35</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D16" s="2">
-        <f>14/(1000*1000*1000)</f>
-        <v>1.4E-8</v>
+        <f>12/(1000*1000*1000)</f>
+        <v>1.2E-8</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
-        <v>6</v>
+      <c r="A17" t="s">
+        <v>36</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D17" s="2">
         <f>14/(1000*1000*1000)</f>
         <v>1.4E-8</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
-        <v>7</v>
+      <c r="A18" t="s">
+        <v>37</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D18" s="2">
-        <f>31/(1000*1000*1000)</f>
-        <v>3.1E-8</v>
+        <f>14/(1000*1000*1000)</f>
+        <v>1.4E-8</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
-        <v>8</v>
+      <c r="A19" t="s">
+        <v>38</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D19" s="2">
         <f>31/(1000*1000*1000)</f>
         <v>3.1E-8</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="4" t="s">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="2">
+        <f>31/(1000*1000*1000)</f>
+        <v>3.1E-8</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20" s="5">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="2">
+        <f>12/(1000*1000*1000)</f>
+        <v>1.2E-8</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="2">
+        <f>14/(1000*1000*1000)</f>
+        <v>1.4E-8</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="2">
+        <f>31/(1000*1000*1000)</f>
+        <v>3.1E-8</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="2">
+        <v>1</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="5">
         <f>(12/50) / (1000*1000*1000)</f>
         <v>2.4E-10</v>
       </c>
-      <c r="E20" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
+      <c r="E25" s="5" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
+      <c r="A26" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="5">
+        <f>(12/50) / (1000*1000*1000)</f>
+        <v>2.4E-10</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
+      <c r="A27" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="5">
+        <f>(12/50) / (1000*1000*1000)</f>
+        <v>2.4E-10</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
+      <c r="A28" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="5">
+        <f>(12/50) / (1000*1000*1000)</f>
+        <v>2.4E-10</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
+      <c r="A29" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="2">
+        <v>1</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
+      <c r="A30" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="5">
+        <f>(12/50) / (1000*1000*1000)</f>
+        <v>2.4E-10</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
+      <c r="A31" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="2">
+        <v>1</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="5">
+        <f>(12/50) / (1000*1000*1000)</f>
+        <v>2.4E-10</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" s="2">
+        <v>1</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" s="2">
+        <v>1</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" s="2">
+        <v>1</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>